<commit_message>
Chargement de l'état initial de la map
</commit_message>
<xml_diff>
--- a/doc/planete/DispositionInitial.xlsx
+++ b/doc/planete/DispositionInitial.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\ENSI\Annee_2\IA\Projet\colonisation_prunier_rabotin_sechi_servat\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\ENSI\Annee_2\IA\Projet\colonisation_prunier_rabotin_sechi_servat\doc\planete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{364D7E7F-1038-4740-BD31-7F3FE6E9F39F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D6BD1A-016E-46C8-AF80-98FBB91BE16A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13665" yWindow="3390" windowWidth="21600" windowHeight="11835" xr2:uid="{1C357A11-E04B-4EF9-AE18-4830828F7EA8}"/>
+    <workbookView xWindow="-13875" yWindow="2130" windowWidth="21600" windowHeight="11835" xr2:uid="{1C357A11-E04B-4EF9-AE18-4830828F7EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>n°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legende </t>
+  </si>
+  <si>
+    <t>BASE</t>
+  </si>
+  <si>
+    <t>ORE</t>
+  </si>
+  <si>
+    <t>WATER</t>
+  </si>
+  <si>
+    <t>BEDROCK</t>
+  </si>
+  <si>
+    <t>FOREST</t>
+  </si>
+  <si>
+    <t>DESERT</t>
+  </si>
+  <si>
+    <t>FOOD</t>
+  </si>
+  <si>
+    <t>OBSTACLE</t>
+  </si>
+  <si>
+    <t>MEADOW_DRY</t>
+  </si>
+  <si>
+    <t>MEADOW_NORMAL</t>
+  </si>
+  <si>
+    <t>MEADOW_GREASY</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,13 +87,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF9876AA"/>
+      <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2B2B2B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,9 +127,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -394,18 +466,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500598CA-2BC1-4DE8-855D-6454916DDDAD}">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V22" sqref="B2:V22"/>
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="23" width="3.7109375" customWidth="1"/>
+    <col min="25" max="25" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>0</v>
@@ -471,319 +544,349 @@
         <v>20</v>
       </c>
       <c r="W1" s="1"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O2" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P2" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q2" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R2" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S2" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T2" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W2" s="1"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1">
+        <v>8</v>
+      </c>
+      <c r="M3" s="1">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1">
+        <v>10</v>
+      </c>
+      <c r="O3" s="1">
+        <v>10</v>
+      </c>
+      <c r="P3" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>10</v>
+      </c>
+      <c r="R3" s="1">
+        <v>8</v>
+      </c>
+      <c r="S3" s="1">
+        <v>8</v>
+      </c>
+      <c r="T3">
+        <v>6</v>
+      </c>
+      <c r="U3" s="1">
+        <v>3</v>
+      </c>
+      <c r="V3" s="1">
+        <v>3</v>
+      </c>
+      <c r="W3" s="1"/>
+      <c r="Y3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z3">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1">
-        <v>1</v>
-      </c>
-      <c r="V3" s="1">
-        <v>1</v>
-      </c>
-      <c r="W3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S4" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W4" s="1"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O5" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P5" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q5" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R5" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S5" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U5" s="1">
-        <v>1</v>
-      </c>
-      <c r="V5" s="1">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="V5">
+        <v>6</v>
       </c>
       <c r="W5" s="1"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
@@ -792,436 +895,472 @@
         <v>0</v>
       </c>
       <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="P6">
+        <v>6</v>
       </c>
       <c r="Q6" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R6" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S6" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6" s="1"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K7" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L7" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M7" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
       </c>
       <c r="P7" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q7" s="1">
-        <v>0</v>
-      </c>
-      <c r="R7" s="1">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="R7">
+        <v>7</v>
       </c>
       <c r="S7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V7" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="W7" s="1"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J8" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K8" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="V8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W8" s="1"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K9" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L9" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M9" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N9" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O9" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P9" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q9" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U9" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="V9" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W9" s="1"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G10" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H10" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I10" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J10" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L10" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N10" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O10" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="P10" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q10" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R10" s="1">
-        <v>0</v>
-      </c>
-      <c r="S10" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="S10">
+        <v>6</v>
       </c>
       <c r="T10" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U10" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="V10" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="W10" s="1"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F11" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H11" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J11" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K11" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M11" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N11" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q11" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R11" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S11" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T11" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U11" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="V11" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="W11" s="1"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
       </c>
       <c r="I12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K12" s="1">
-        <v>0</v>
-      </c>
-      <c r="L12" s="1">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
       </c>
       <c r="M12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O12" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P12" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q12" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R12" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S12" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T12" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U12" s="1">
         <v>0</v>
@@ -1230,64 +1369,70 @@
         <v>0</v>
       </c>
       <c r="W12" s="1"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G13" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I13" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N13" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O13" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P13" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q13" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R13" s="1">
         <v>0</v>
       </c>
       <c r="S13" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T13" s="1">
         <v>0</v>
@@ -1296,232 +1441,232 @@
         <v>0</v>
       </c>
       <c r="V13" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H14" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I14" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J14" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K14" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L14" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M14" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N14" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O14" s="1">
-        <v>0</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="P14">
+        <v>6</v>
       </c>
       <c r="Q14" s="1">
         <v>0</v>
       </c>
       <c r="R14" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S14" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T14" s="1">
         <v>0</v>
       </c>
       <c r="U14" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V14" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I15" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>6</v>
       </c>
       <c r="L15" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M15" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="N15" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O15" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="P15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="Q15">
+        <v>6</v>
       </c>
       <c r="R15" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S15" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T15" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U15" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V15" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J16" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K16" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L16" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O16" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="P16" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q16" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R16" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S16" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T16" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U16" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V16" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
       </c>
       <c r="E17" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1530,286 +1675,286 @@
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
       </c>
       <c r="J17" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K17" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L17" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M17" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N17" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O17" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P17" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q17" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R17" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S17" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T17" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U17" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="V17" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="W17" s="1"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E18" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F18" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G18" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H18" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I18" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J18" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K18" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L18" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M18" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N18" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O18" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P18" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q18" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R18" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S18" s="1">
-        <v>0</v>
-      </c>
-      <c r="T18" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="T18">
+        <v>6</v>
       </c>
       <c r="U18" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V18" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W18" s="1"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D19" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E19" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F19" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L19" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M19" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N19" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R19" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S19" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T19" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U19" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="V19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W19" s="1"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D20" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F20" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G20" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H20" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I20" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J20" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K20" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L20" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M20" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N20" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O20" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P20" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q20" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R20" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S20" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W20" s="1"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H21" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I21" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
@@ -1818,110 +1963,110 @@
         <v>0</v>
       </c>
       <c r="L21" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M21" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N21" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O21" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P21" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q21" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S21" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T21" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W21" s="1"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
       </c>
       <c r="H22" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I22" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J22" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K22" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L22" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M22" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N22" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O22" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P22" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q22" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R22" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W22" s="1"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1947,9 +2092,10 @@
       <c r="W23" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:W23">
+  <conditionalFormatting sqref="F5:G5 G4 L3 O2:Q2 B6:H6 B9:J9 C10:I10 K10:Q10 B12:C12 L11 O11:P11 Q13 Q12:R12 T12 U10:W11 W8:W9 R9 U8 Q7 Q6:S6 S5:U5 P3 R3:S3 S2:W2 V17:W17 W16 T17 U18:W18 B19:K19 B23:W23 R22 C21:D21 B22:C22 Q20:S20 C20:H20 M19:R19 J18:P18 M17:R17 M16:U16 N15:P15 L15 L14:O14 I14 H13:J13 F18:G18 B18:C18 B13:B15 D14 E13 E12:G12 B11 D11:I11 C8:G8 B7:C7 E7:G7 I7:K8 I22:K22 L21 J20 D3:F3 F2 C4:C5 F14:G14 L12:N13 R14:S14 S13 U14:W14 V13:W13 W12 T9 V7:W7 S4:T4 V4:W4 T19:U19 R21:T21 W19:W22 J6:K6 R15:W15 U3:W3 W5:W6 E15 I12:J12 K4:K5">
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>